<commit_message>
Modifications due to how-to 549.
</commit_message>
<xml_diff>
--- a/NothWesternStates.xlsx
+++ b/NothWesternStates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\GitLab\examples\application-examples\contract-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834BD56E-955D-429B-9DD0-ED8B33CFEF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7860125-6866-4CDF-AF14-5B02DB2110A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="2100" windowWidth="21600" windowHeight="11295" xr2:uid="{35D11483-C57D-4FF9-9C80-BE782F469030}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35D11483-C57D-4FF9-9C80-BE782F469030}"/>
   </bookViews>
   <sheets>
     <sheet name="Producers" sheetId="1" r:id="rId1"/>
@@ -456,7 +456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2878F2E8-55E5-45EC-A393-38ED5A80DE1F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -542,15 +542,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99407143-3B12-43B4-BAF4-3A5D9F203278}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>100</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>65</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>70</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -616,7 +616,7 @@
         <v>120</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>60</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -638,7 +638,7 @@
         <v>75</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>95</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding new information into results page, deleting unrelevant stuff, changing translations.
</commit_message>
<xml_diff>
--- a/NothWesternStates.xlsx
+++ b/NothWesternStates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\GitLab\examples\application-examples\contract-allocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7860125-6866-4CDF-AF14-5B02DB2110A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB7E29F-BE48-43C2-8E5C-CC1562BCC0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{35D11483-C57D-4FF9-9C80-BE782F469030}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{35D11483-C57D-4FF9-9C80-BE782F469030}"/>
   </bookViews>
   <sheets>
     <sheet name="Producers" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="23">
   <si>
     <t>Seattle</t>
   </si>
@@ -99,10 +99,13 @@
     <t>Minimal Delivery</t>
   </si>
   <si>
-    <t>Contract Size</t>
-  </si>
-  <si>
     <t>Minimal Number of Contributors</t>
+  </si>
+  <si>
+    <t>Minimum Contract Size</t>
+  </si>
+  <si>
+    <t>Maximum Contract Size</t>
   </si>
 </sst>
 </file>
@@ -540,142 +543,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99407143-3B12-43B4-BAF4-3A5D9F203278}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
         <v>100</v>
       </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
         <v>65</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4">
+        <v>50</v>
+      </c>
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5">
+        <v>35</v>
+      </c>
+      <c r="C5">
         <v>70</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
         <v>120</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
         <v>60</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8">
+        <v>30</v>
+      </c>
+      <c r="C8">
         <v>75</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9">
+        <v>50</v>
+      </c>
+      <c r="C9">
         <v>100</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10">
         <v>95</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11">
+        <v>40</v>
+      </c>
+      <c r="C11">
         <v>85</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>